<commit_message>
feat: upload actual data
</commit_message>
<xml_diff>
--- a/input/key.xlsx
+++ b/input/key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\water-taste-test\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD43C88-C716-4625-A1D0-9767B2DC188F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E77C0-412A-4DF0-8550-9B25A2A08548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25635" windowHeight="20505" xr2:uid="{9B3C4830-F8AE-4EBF-9410-A8980EAFB3CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{9B3C4830-F8AE-4EBF-9410-A8980EAFB3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>water</t>
   </si>
@@ -59,19 +59,22 @@
     <t>E</t>
   </si>
   <si>
-    <t>PUP Fountain</t>
-  </si>
-  <si>
-    <t>Tas Well Water</t>
-  </si>
-  <si>
     <t>Fiji</t>
   </si>
   <si>
-    <t>Dasani</t>
-  </si>
-  <si>
-    <t>CSV Generic</t>
+    <t>Well Water</t>
+  </si>
+  <si>
+    <t>Evian</t>
+  </si>
+  <si>
+    <t>Smart Water</t>
+  </si>
+  <si>
+    <t>Press Building Water</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -443,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5905C8-1431-4047-8469-C338C3E07DC2}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,31 +462,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -491,12 +494,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>